<commit_message>
feat: implement category filtering in pipeline with detailed merge statistics and source tracking
Add merge_with_category_filter and merge_with_category_filter_and_stats methods (286 lines) to DataMergerNewFormat for category-aware merging with source tracking and last_updated timestamps. Update PipelineNewFormat.run and run_with_stats to accept selected_categories parameter and use new merge methods when categories provided. Replace xmlFeedName with source column throughout XMLParserNewFormat for
</commit_message>
<xml_diff>
--- a/tests/test_data/all_steps_output.xlsx
+++ b/tests/test_data/all_steps_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EH2"/>
+  <dimension ref="A1:EI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>xmlFeedName</t>
+          <t>source</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
@@ -1122,6 +1122,11 @@
       <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>aiProcessedDate</t>
+        </is>
+      </c>
+      <c r="EI1" s="1" t="inlineStr">
+        <is>
+          <t>last_updated</t>
         </is>
       </c>
     </row>
@@ -1432,6 +1437,7 @@
       <c r="EF2" t="inlineStr"/>
       <c r="EG2" t="inlineStr"/>
       <c r="EH2" t="inlineStr"/>
+      <c r="EI2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add namespace support and configurable root element handling to Gastromarket XML parser
Add namespace registration and prefix handling for XML parsing with configurable namespace URL from feed config. Update root element extraction to use configurable root_element (default "channel") instead of hardcoded structure. Modify element finding logic to use namespace prefix ("g:") when namespace_url is configured, enabling proper parsing of namespaced XML feeds. Change default item_element from "PRODUKT" to "item
</commit_message>
<xml_diff>
--- a/tests/test_data/all_steps_output.xlsx
+++ b/tests/test_data/all_steps_output.xlsx
@@ -1160,11 +1160,7 @@
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>GM Manufacturer</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
@@ -1198,12 +1194,12 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>Tovary a kategórie &gt; GM Category &gt; Subcategory</t>
+          <t>Tovary a kategórie &gt; GM Category | Subcategory</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>Tovary a kategórie &gt; GM Category &gt; Subcategory</t>
+          <t>Tovary a kategórie &gt; GM Category | Subcategory</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">

</xml_diff>